<commit_message>
Updated 3D Model Directory for the backplane
</commit_message>
<xml_diff>
--- a/PCB-1-2/Files for Production/BOM & CSV/JLCPCB -1_-2.xlsx
+++ b/PCB-1-2/Files for Production/BOM & CSV/JLCPCB -1_-2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erick29\Downloads\UpdatedPCB\PCB-1-2\Files for Production\BOM &amp; CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devin\Documents\ACDC_PCBFiles\PCB-1-2\Files for Production\BOM &amp; CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EAAAB3-6F00-4FC6-9D78-B59839B50D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97AB964-9E9F-40F6-B3F4-8445A0502FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -854,10 +854,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1179,20 +1175,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:4" ht="15.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2121,12 +2117,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f0ce7fdb-ba90-47a1-b35b-9382e1297453" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="42c5bc0e-8e1e-48d7-bb43-c22d7a2fad61">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2337,20 +2335,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f0ce7fdb-ba90-47a1-b35b-9382e1297453" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="42c5bc0e-8e1e-48d7-bb43-c22d7a2fad61">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ED1393E-2924-4618-9258-D126E54FAC7F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04DCC733-33B7-49A3-8837-351E13C65588}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="42c5bc0e-8e1e-48d7-bb43-c22d7a2fad61"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f0ce7fdb-ba90-47a1-b35b-9382e1297453"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2375,18 +2380,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04DCC733-33B7-49A3-8837-351E13C65588}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2ED1393E-2924-4618-9258-D126E54FAC7F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="42c5bc0e-8e1e-48d7-bb43-c22d7a2fad61"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f0ce7fdb-ba90-47a1-b35b-9382e1297453"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>